<commit_message>
add base de datos.txt
</commit_message>
<xml_diff>
--- a/Usuarios.xlsx
+++ b/Usuarios.xlsx
@@ -19,7 +19,7 @@
     <t xml:space="preserve"> Buenos días </t>
   </si>
   <si>
-    <t xml:space="preserve"> Anexo formulario ingreso poliza exequias del mes de Agosto2021 </t>
+    <t xml:space="preserve"> Anexo formulario ingreso poliza exequias del mes de Agosto2022</t>
   </si>
   <si>
     <t>Id</t>
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2">
-        <v>44574.09762678241</v>
+        <v>44574.60294081019</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>